<commit_message>
rerun the analysis scripts
</commit_message>
<xml_diff>
--- a/Study 1/results/INTBRSCI_ml_results.xlsx
+++ b/Study 1/results/INTBRSCI_ml_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">rowname</t>
   </si>
@@ -30,6 +30,12 @@
   </si>
   <si>
     <t xml:space="preserve">p.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ci.lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ci.upper</t>
   </si>
   <si>
     <t xml:space="preserve">r_xy1y2</t>
@@ -455,10 +461,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
         <v>0.421187035774277</v>
@@ -475,10 +487,16 @@
       <c r="F2" t="n">
         <v>0.00226701817625697</v>
       </c>
+      <c r="G2" t="n">
+        <v>0.158405518943659</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.683968552604894</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
         <v>0.0145306979210766</v>
@@ -495,10 +513,16 @@
       <c r="F3" t="n">
         <v>0.648279540235665</v>
       </c>
+      <c r="G3" t="n">
+        <v>-0.0491117252880285</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.0781731211301816</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>-0.0199519994936245</v>
@@ -515,10 +539,16 @@
       <c r="F4" t="n">
         <v>0.565337326046853</v>
       </c>
+      <c r="G4" t="n">
+        <v>-0.0892414740387267</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0493374750514777</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>0.066100859848457</v>
@@ -535,10 +565,16 @@
       <c r="F5" t="n">
         <v>0.648279540235665</v>
       </c>
+      <c r="G5" t="n">
+        <v>-0.223411654953692</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.355613374650606</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>-0.0833499466259191</v>
@@ -555,10 +591,16 @@
       <c r="F6" t="n">
         <v>0.565337326046853</v>
       </c>
+      <c r="G6" t="n">
+        <v>-0.37280835438689</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.206108461135052</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
         <v>0.0632866772436911</v>
@@ -575,10 +617,16 @@
       <c r="F7" t="n">
         <v>0.648279540235665</v>
       </c>
+      <c r="G7" t="n">
+        <v>-0.213900111616524</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.340473466103907</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
         <v>-0.0868984930508933</v>
@@ -595,10 +643,16 @@
       <c r="F8" t="n">
         <v>0.565337326046853</v>
       </c>
+      <c r="G8" t="n">
+        <v>-0.388680323196871</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.214883337095084</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="n">
         <v>-0.00271065078627396</v>
@@ -615,10 +669,16 @@
       <c r="F9" t="n">
         <v>0.934185856338452</v>
       </c>
+      <c r="G9" t="n">
+        <v>-0.0683621159675101</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0629408143949622</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" t="n">
         <v>0.208364528759494</v>
@@ -635,10 +695,16 @@
       <c r="F10" t="n">
         <v>0.00000000000000000000000129353175786456</v>
       </c>
+      <c r="G10" t="n">
+        <v>0.187264191354415</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.229464866164573</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="n">
         <v>0.0344826974147011</v>
@@ -655,10 +721,16 @@
       <c r="F11" t="n">
         <v>0.00226701817625697</v>
       </c>
+      <c r="G11" t="n">
+        <v>0.0129687030098434</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0559966918195587</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" t="n">
         <v>0.15048959593645</v>
@@ -667,10 +739,12 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" t="n">
         <v>0.149741156866595</v>
@@ -679,10 +753,12 @@
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" t="n">
         <v>-6.04258205944936</v>
@@ -691,10 +767,12 @@
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15" t="n">
         <v>0.0317720466284271</v>
@@ -711,10 +789,16 @@
       <c r="F15" t="n">
         <v>0.318886228341874</v>
       </c>
+      <c r="G15" t="n">
+        <v>-0.0316463739617981</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0951904672186524</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" t="n">
         <v>0.138379262390983</v>
@@ -731,10 +815,16 @@
       <c r="F16" t="n">
         <v>0.318886228341874</v>
       </c>
+      <c r="G16" t="n">
+        <v>-0.137831910465116</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.414590435247082</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B17" t="n">
         <v>0.140826263085645</v>
@@ -751,10 +841,16 @@
       <c r="F17" t="n">
         <v>0.349949773489855</v>
       </c>
+      <c r="G17" t="n">
+        <v>-0.159124364439563</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.440776890610853</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" t="n">
         <v>0.0290613958421532</v>
@@ -771,10 +867,16 @@
       <c r="F18" t="n">
         <v>0.324139770117833</v>
       </c>
+      <c r="G18" t="n">
+        <v>-0.0982234505760569</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.156346242260363</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B19" t="n">
         <v>0.126573354487382</v>
@@ -791,10 +893,16 @@
       <c r="F19" t="n">
         <v>0.324139770117833</v>
       </c>
+      <c r="G19" t="n">
+        <v>-0.427800223233049</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.680946932207813</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" t="n">
         <v>0.132201719696914</v>
@@ -811,10 +919,16 @@
       <c r="F20" t="n">
         <v>0.324139770117833</v>
       </c>
+      <c r="G20" t="n">
+        <v>-0.446823309907384</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.711226749301211</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="n">
         <v>0.0344826974147011</v>
@@ -831,10 +945,16 @@
       <c r="F21" t="n">
         <v>0.00113350908812848</v>
       </c>
+      <c r="G21" t="n">
+        <v>0.0129687030098434</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0559966918195587</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" t="n">
         <v>0.00542130157254793</v>
@@ -851,10 +971,16 @@
       <c r="F22" t="n">
         <v>0.467092928169226</v>
       </c>
+      <c r="G22" t="n">
+        <v>-0.125881628789924</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.13672423193502</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" t="n">
         <v>0.150185170294584</v>
@@ -871,10 +997,16 @@
       <c r="F23" t="n">
         <v>0.00113350908812848</v>
       </c>
+      <c r="G23" t="n">
+        <v>0.0564835994878654</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.243886741101303</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" t="n">
         <v>0.0236118158072022</v>
@@ -891,10 +1023,16 @@
       <c r="F24" t="n">
         <v>0.467092928169226</v>
       </c>
+      <c r="G24" t="n">
+        <v>-0.548262034997135</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.59548566661154</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25" t="n">
         <v>0.149450806474376</v>
@@ -911,10 +1049,16 @@
       <c r="F25" t="n">
         <v>0.000856296845304875</v>
       </c>
+      <c r="G25" t="n">
+        <v>0.0589385086387653</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.239963104309987</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26" t="n">
         <v>0.0172490867774621</v>
@@ -930,6 +1074,12 @@
       </c>
       <c r="F26" t="n">
         <v>0.475946892438454</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-0.554614093318411</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.589112266873336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>